<commit_message>
capacity for circuit, potential for solar language change, client-side simplified excel js, updated images
</commit_message>
<xml_diff>
--- a/download/institutional_sites_metadata.xlsx
+++ b/download/institutional_sites_metadata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B324E5D-D0AE-4548-AC94-E33794BCB986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F917E178-35D5-48E2-93B4-44D873C5E760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,24 +235,12 @@
     <t>Proportion of geometry located within the zip code</t>
   </si>
   <si>
-    <t>Low level estimate of available parking lot area annual solar PV generation capacity potential (MWh AC)</t>
-  </si>
-  <si>
-    <t>High level estimate of available parking lot area annual solar PV generation capacity potential (MWh AC)</t>
-  </si>
-  <si>
     <t>Rooftop tolar annual solar PV generation capacity (MWh AC) (Los Angeles County Solar Map)</t>
   </si>
   <si>
     <t>Total residential electricity usage (kWh) per capita within census block group (UCLA Energy Atlas)</t>
   </si>
   <si>
-    <t>Combine total of the low estimate of parking lot and rooftop generation capacity potential (MWh AC)</t>
-  </si>
-  <si>
-    <t>Combine total of the high estimate of parking lot and rooftop generation capacity potential (MWh AC)</t>
-  </si>
-  <si>
     <t>CalEnviroScreen 3.0 Percentile</t>
   </si>
   <si>
@@ -316,28 +304,40 @@
     <t>System name defined by Southern California Edison (SCE), linked by nearest distribution circuit</t>
   </si>
   <si>
-    <t>15% Penetration Capacity (MW-AC)</t>
-  </si>
-  <si>
     <t>Existing in front of the meter solar generation (MW-AC)</t>
   </si>
   <si>
-    <t>Rooftop solar generation capacity potential (MW-AC)</t>
-  </si>
-  <si>
-    <t>Low level estimate of available parking lot area solar PV generation capacity potential (MW-AC)</t>
-  </si>
-  <si>
-    <t>High level estimate of available parking lot area solar PV generation capacity potential (MW-AC)</t>
-  </si>
-  <si>
-    <t>Combined total of the low estimate of parking lot generation potential and rooftop solar generation capacity potential (MW-AC)</t>
-  </si>
-  <si>
-    <t>Combined total of the high estimate of parking lot generation potential and rooftop solar generation capacity potential (MW-AC)</t>
-  </si>
-  <si>
     <t>Parking lot area (sqft) suitable for solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15% Penetration Capacity (MW-AC) of the circuit serving the site. Importance dictated by Rule 21, the total combined nameplate capacity of all generation assets connected to each distribution circuit must not exceed 15% of the historical maximum load experienced on that circuit over the previous 18 months. </t>
+  </si>
+  <si>
+    <t>Combine total of the low estimate of parking lot and rooftop solar nameplate generation potential (MWh AC)</t>
+  </si>
+  <si>
+    <t>Combine total of the high estimate of parking lot and rooftop solar nameplate generation potential (MWh AC)</t>
+  </si>
+  <si>
+    <t>Low level estimate of available parking lot area solar PV nameplate solar generation  potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>Rooftop solar nameplate solar generation potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>High level estimate of available parking lot area solar PV nameplate solar generation  potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>Low level estimate of available parking lot area annual solar PV generation potential (MWh AC)</t>
+  </si>
+  <si>
+    <t>High level estimate of available parking lot area annual solar PV generation potential (MWh AC)</t>
+  </si>
+  <si>
+    <t>Combined total of the low estimate of parking lot generation potential and rooftop solar generation potential (MW-AC)</t>
+  </si>
+  <si>
+    <t>Combined total of the high estimate of parking lot generation potential and rooftop solar generation potential (MW-AC)</t>
   </si>
 </sst>
 </file>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,15 +728,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -848,7 +848,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -904,7 +904,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -984,7 +984,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,7 +992,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1040,7 +1040,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,7 +1048,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>